<commit_message>
25/07 added quick launch
</commit_message>
<xml_diff>
--- a/media/output/result/Production_Ncomplex_evaluation_weighted_edit_distance0.0,0.0,1.0.xlsx
+++ b/media/output/result/Production_Ncomplex_evaluation_weighted_edit_distance0.0,0.0,1.0.xlsx
@@ -656,10 +656,10 @@
         <v>0</v>
       </c>
       <c r="E8" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F8" t="n">
-        <v>12</v>
+        <v>0</v>
       </c>
       <c r="G8" t="n">
         <v>0</v>
@@ -685,10 +685,10 @@
         <v>0</v>
       </c>
       <c r="E9" t="n">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="F9" t="n">
-        <v>11</v>
+        <v>0</v>
       </c>
       <c r="G9" t="n">
         <v>0</v>
@@ -714,10 +714,10 @@
         <v>0</v>
       </c>
       <c r="E10" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="F10" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="G10" t="n">
         <v>0</v>

</xml_diff>